<commit_message>
Add expand_term & create event dict Add unit tests
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarrahi_mm/Documents/SUT/8 Modern Information Retrieval/SUT_MIR_C1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jafarinegin/PycharmProjects/SUT_MIR_C1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F42FF6-CC64-014B-8BF7-256688368F35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E1DAC-7D3C-4949-907B-B0204F597246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4120" yWindow="4860" windowWidth="36500" windowHeight="16940" xr2:uid="{D36F0CFF-FA29-1544-8A2A-7FC57DF3D724}"/>
+    <workbookView xWindow="0" yWindow="800" windowWidth="30720" windowHeight="16940" xr2:uid="{D36F0CFF-FA29-1544-8A2A-7FC57DF3D724}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -50,24 +50,12 @@
     <t>شخصیت</t>
   </si>
   <si>
-    <t>#NUM (درصد|واحد)؟ افزایش سرمایه</t>
-  </si>
-  <si>
-    <t>#NUM؟ (درصد|واحد)؟ (ضرر|سود)</t>
-  </si>
-  <si>
     <t>افزایش سرمایه</t>
   </si>
   <si>
-    <t>(اطلاعیه ی؟|آگهی|اعلامیه)؟ ((افشای؟ (اطلاعات)؟ (الف|ب|با اهمیت))|ثبت افزایش سرمایه|صورت (های)؟ مالی|فعالیت ماهانه|دعوت به مجمع (عمومی|عادی|)|پذیره نویسی عمومی)</t>
-  </si>
-  <si>
     <t>تقسیم سود</t>
   </si>
   <si>
-    <t>دامنه ی؟ نوسان</t>
-  </si>
-  <si>
     <t>دامنه نوسان</t>
   </si>
   <si>
@@ -80,9 +68,6 @@
     <t>صفت سهم</t>
   </si>
   <si>
-    <t>#NUM؟ (درصد|واحد)؟ (تاثیر)؟ (مثبت|منفی)</t>
-  </si>
-  <si>
     <t>سود/ضرر</t>
   </si>
   <si>
@@ -96,6 +81,21 @@
   </si>
   <si>
     <t>گزارش</t>
+  </si>
+  <si>
+    <t>(#NUM )؟(درصد |واحد )؟(ضرر|سود)</t>
+  </si>
+  <si>
+    <t>#NUM (درصد |واحد )؟افزایش سرمایه</t>
+  </si>
+  <si>
+    <t>دامنه (ی )؟نوسان</t>
+  </si>
+  <si>
+    <t>(#NUM )؟(درصد |واحد )؟(تاثیر )؟(مثبت|منفی)</t>
+  </si>
+  <si>
+    <t>(اطلاعیه (ی )؟|آگهی |اعلامیه )؟((افشا (ی )؟(اطلاعات )؟(الف|ب|با اهمیت))|ثبت افزایش سرمایه|صورت (ها ی )؟مالی|فعالیت ماهانه|دعوت به مجمع( عمومی| عادی)؟|پذیره نویسی عمومی)</t>
   </si>
 </sst>
 </file>
@@ -464,7 +464,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,15 +483,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -507,58 +507,58 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
         <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add many forms ...
</commit_message>
<xml_diff>
--- a/events.xlsx
+++ b/events.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jafarinegin/PycharmProjects/SUT_MIR_C1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jarrahi_mm/Documents/SUT/8 Modern Information Retrieval/SUT_MIR_C1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459E1DAC-7D3C-4949-907B-B0204F597246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC77A344-D1CF-A14C-B357-A1E5321F8F52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="800" windowWidth="30720" windowHeight="16940" xr2:uid="{D36F0CFF-FA29-1544-8A2A-7FC57DF3D724}"/>
+    <workbookView xWindow="1040" yWindow="-20240" windowWidth="31660" windowHeight="17660" xr2:uid="{D36F0CFF-FA29-1544-8A2A-7FC57DF3D724}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>اطلاعیه</t>
   </si>
@@ -59,9 +59,6 @@
     <t>دامنه نوسان</t>
   </si>
   <si>
-    <t>نوسان شدید</t>
-  </si>
-  <si>
     <t>سهم (رانتی|خوب|بد|آشغال)</t>
   </si>
   <si>
@@ -77,18 +74,12 @@
     <t>رشد سهم</t>
   </si>
   <si>
-    <t>گزارش فعالیت (ماهانه|فصلی|سالانه)</t>
-  </si>
-  <si>
     <t>گزارش</t>
   </si>
   <si>
     <t>(#NUM )؟(درصد |واحد )؟(ضرر|سود)</t>
   </si>
   <si>
-    <t>#NUM (درصد |واحد )؟افزایش سرمایه</t>
-  </si>
-  <si>
     <t>دامنه (ی )؟نوسان</t>
   </si>
   <si>
@@ -96,6 +87,42 @@
   </si>
   <si>
     <t>(اطلاعیه (ی )؟|آگهی |اعلامیه )؟((افشا (ی )؟(اطلاعات )؟(الف|ب|با اهمیت))|ثبت افزایش سرمایه|صورت (ها ی )؟مالی|فعالیت ماهانه|دعوت به مجمع( عمومی| عادی)؟|پذیره نویسی عمومی)</t>
+  </si>
+  <si>
+    <t>بازگشایی</t>
+  </si>
+  <si>
+    <t>(#NUM درصد |#NUM واحد )؟افزایش سرمایه</t>
+  </si>
+  <si>
+    <t>صف</t>
+  </si>
+  <si>
+    <t>روند</t>
+  </si>
+  <si>
+    <t>صف( خرید| فروش)</t>
+  </si>
+  <si>
+    <t>روند( صعودی| نزولی)</t>
+  </si>
+  <si>
+    <t>ریزش</t>
+  </si>
+  <si>
+    <t>گزارش( فعالیت)؟ (ماهانه|فصلی|سالانه|#NUM ماهه)</t>
+  </si>
+  <si>
+    <t>تکنیکال</t>
+  </si>
+  <si>
+    <t>نوسان( شدید)؟</t>
+  </si>
+  <si>
+    <t>(کندل|پول بک|ابر کومو|دو قلو|سقف|کف سازی|کف|سر و شانه|مکدی|کراس|حمایت|مقاومت|آر اس آی|کد به کد)</t>
+  </si>
+  <si>
+    <t>توقف نماد</t>
   </si>
 </sst>
 </file>
@@ -461,10 +488,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC6843B9-ACD7-D047-BCB9-D51EA433A5CE}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="169" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -483,15 +510,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B3" t="s">
         <v>0</v>
@@ -507,7 +534,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -523,7 +550,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -531,34 +558,82 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>